<commit_message>
creando excel BOLSAS Total
</commit_message>
<xml_diff>
--- a/excel/monica.xlsx
+++ b/excel/monica.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
   <si>
     <t>AGUILAS</t>
   </si>
@@ -655,8 +655,8 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
       </c>
       <c r="F1" s="6">
         <f>F40</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1124,8 +1124,8 @@
       <c r="E27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="3">
-        <v>1</v>
+      <c r="F27" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1335,7 +1335,7 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F40" s="7">
         <f>SUM(F2:F39)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>